<commit_message>
Got the first part of the controls stage done, player is now prompted to use WASD. Dialogue boxes can now fade out, and distinguish between tween in duration and tween out duration, and can opt to fade or tween out, or both or neither. Got stuck on the fading out because I forgot to adjust some in-code variables passed to DialogueBox on submitting dialogue.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB6EF9A4-FDC8-4C9F-B465-716AEDC45118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2A4AFAB-9C0C-4269-9BA8-598A8D079209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial Dialogue" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="P.O.Ds_first_steps">'Tutorial Dialogue'!$B$2:$F$18</definedName>
+    <definedName name="P.O.Ds_first_steps">'Tutorial Dialogue'!$B$2:$F$22</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="160">
   <si>
     <t>Stage</t>
   </si>
@@ -692,6 +692,42 @@
   </si>
   <si>
     <t>You don't need to put dialogue in quotation marks unless the character is using them in-line. Just type it as you want it presented in the dialogue box excepting the special characters for line breaks and colour tags.</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Press W</t>
+  </si>
+  <si>
+    <t>Press A</t>
+  </si>
+  <si>
+    <t>Press S</t>
+  </si>
+  <si>
+    <t>Press D</t>
   </si>
 </sst>
 </file>
@@ -795,7 +831,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -844,6 +880,18 @@
         <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8ED7DD"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8ED7DD"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -857,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -937,6 +985,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -962,6 +1020,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF8ED7DD"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FF00FF00"/>
     </mruColors>
@@ -1179,11 +1238,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB979"/>
+  <dimension ref="A1:AB983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1252,93 +1311,97 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>14</v>
+      <c r="B4" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>152</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6"/>
+      <c r="B6" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>158</v>
+      </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="B7" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>6</v>
+      <c r="B8" s="37" t="s">
+        <v>13</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
@@ -1348,58 +1411,62 @@
         <v>6</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>30</v>
+      <c r="B10" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>122</v>
+        <v>22</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="10"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>30</v>
+      <c r="B11" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>123</v>
+        <v>24</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>30</v>
+      <c r="B12" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>124</v>
+        <v>26</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>27</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
@@ -1412,33 +1479,29 @@
         <v>6</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>6</v>
+      <c r="B14" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
@@ -1448,10 +1511,10 @@
         <v>30</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
@@ -1460,169 +1523,141 @@
       <c r="A16" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>6</v>
+      <c r="B16" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>13</v>
+      <c r="B17" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E17" s="6"/>
       <c r="F17" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>30</v>
+      <c r="B18" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="F18" s="9" t="s">
-        <v>46</v>
+      <c r="F18" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>47</v>
+      <c r="A19" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="8"/>
+        <v>125</v>
+      </c>
+      <c r="E19" s="6"/>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>30</v>
+      <c r="A20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="F20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
+      <c r="F20" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>6</v>
+      <c r="A21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="9" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
-        <v>47</v>
+      <c r="A22" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="21" t="s">
-        <v>6</v>
+      <c r="B23" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
@@ -1632,33 +1667,55 @@
         <v>30</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>56</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="6"/>
       <c r="F24" s="7" t="s">
-        <v>57</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>30</v>
+      <c r="B25" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="7"/>
+        <v>50</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
@@ -1668,32 +1725,34 @@
         <v>30</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" s="8"/>
+        <v>129</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="F26" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>30</v>
+      <c r="B27" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="7" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
@@ -1704,14 +1763,16 @@
         <v>30</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E28" s="8"/>
+        <v>130</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F28" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
@@ -1722,13 +1783,13 @@
         <v>30</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="34" t="s">
-        <v>135</v>
+        <v>58</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
@@ -1738,13 +1799,15 @@
         <v>30</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>136</v>
+        <v>59</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="E30" s="8"/>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
@@ -1754,14 +1817,14 @@
         <v>30</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>137</v>
+        <v>61</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
@@ -1772,14 +1835,14 @@
         <v>30</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1790,98 +1853,98 @@
         <v>30</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C38" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D38" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="9" t="s">
+      <c r="E38" s="5"/>
+      <c r="F38" s="9" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1892,88 +1955,82 @@
         <v>6</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="11" t="s">
-        <v>40</v>
+        <v>73</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="23" t="s">
-        <v>76</v>
+      <c r="B40" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="16" t="s">
-        <v>6</v>
+      <c r="B41" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>85</v>
+        <v>140</v>
       </c>
       <c r="E41" s="8"/>
-      <c r="F41" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="23" t="s">
         <v>76</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>143</v>
+        <v>78</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>141</v>
       </c>
       <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
+      <c r="F42" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="18" t="s">
-        <v>13</v>
+      <c r="B43" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>89</v>
+        <v>80</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1984,13 +2041,17 @@
         <v>76</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="7"/>
+        <v>142</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
@@ -2000,51 +2061,51 @@
         <v>6</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E45" s="8"/>
-      <c r="F45" s="9" t="s">
+      <c r="F45" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="18" t="s">
-        <v>13</v>
+      <c r="B46" s="25" t="s">
+        <v>76</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>96</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="23" t="s">
-        <v>76</v>
+      <c r="B47" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
@@ -2054,10 +2115,10 @@
         <v>76</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="7"/>
@@ -2070,103 +2131,109 @@
         <v>6</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>98</v>
+        <v>91</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="E49" s="8"/>
-      <c r="F49" s="7"/>
+      <c r="F49" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="26" t="s">
-        <v>99</v>
+      <c r="A50" s="22" t="s">
+        <v>71</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
+        <v>93</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="B51" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="C51" s="28"/>
-      <c r="D51" s="13"/>
+      <c r="A51" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>145</v>
+      </c>
       <c r="E51" s="8"/>
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="B52" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="C52" s="28" t="s">
-        <v>103</v>
+      <c r="A52" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>105</v>
+      <c r="A53" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="E54" s="8"/>
-      <c r="F54" s="7"/>
+      <c r="A54" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>107</v>
-      </c>
+      <c r="C55" s="28"/>
+      <c r="D55" s="13"/>
       <c r="E55" s="8"/>
       <c r="F55" s="7"/>
     </row>
@@ -2174,14 +2241,14 @@
       <c r="A56" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="28" t="s">
         <v>102</v>
       </c>
       <c r="C56" s="28" t="s">
         <v>103</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="7"/>
@@ -2197,7 +2264,7 @@
         <v>103</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="7"/>
@@ -2213,7 +2280,7 @@
         <v>103</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="7"/>
@@ -2225,27 +2292,27 @@
       <c r="B59" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="15" t="s">
-        <v>110</v>
+      <c r="C59" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="27" t="s">
+      <c r="B60" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="27" t="s">
-        <v>110</v>
+      <c r="C60" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>147</v>
+        <v>108</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="7"/>
@@ -2257,14 +2324,14 @@
       <c r="B61" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C61" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>112</v>
+      <c r="C61" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="E61" s="8"/>
-      <c r="F61" s="9"/>
+      <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
@@ -2273,47 +2340,83 @@
       <c r="B62" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E62" s="8"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E63" s="8"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C64" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E64" s="8"/>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="9"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D62" s="12" t="s">
+      <c r="D66" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E62" s="8"/>
-      <c r="F62" s="9"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="29"/>
-      <c r="B63" s="29"/>
-      <c r="C63" s="29"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="30"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="4"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="30"/>
-      <c r="B65" s="30"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="4"/>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="30"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="4"/>
-      <c r="F66" s="2"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="9"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="30"/>
-      <c r="B67" s="30"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="4"/>
-      <c r="F67" s="2"/>
+      <c r="A67" s="29"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="30"/>
@@ -8699,15 +8802,43 @@
       <c r="D979" s="4"/>
       <c r="F979" s="2"/>
     </row>
+    <row r="980" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A980" s="30"/>
+      <c r="B980" s="30"/>
+      <c r="C980" s="30"/>
+      <c r="D980" s="4"/>
+      <c r="F980" s="2"/>
+    </row>
+    <row r="981" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A981" s="30"/>
+      <c r="B981" s="30"/>
+      <c r="C981" s="30"/>
+      <c r="D981" s="4"/>
+      <c r="F981" s="2"/>
+    </row>
+    <row r="982" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A982" s="30"/>
+      <c r="B982" s="30"/>
+      <c r="C982" s="30"/>
+      <c r="D982" s="4"/>
+      <c r="F982" s="2"/>
+    </row>
+    <row r="983" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A983" s="30"/>
+      <c r="B983" s="30"/>
+      <c r="C983" s="30"/>
+      <c r="D983" s="4"/>
+      <c r="F983" s="2"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AB1">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A35:A49">
+  <conditionalFormatting sqref="A39:A53">
     <cfRule type="containsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(A35))=0</formula>
+      <formula>LEN(TRIM(A39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>

<commit_message>
* Updated StageControl, and the UI and StageManager prefabs to the point where the first section of the tutorial is just about done. * Updating UIElementStatusController to allow me to control some UI elements' interactability and visibility from the game stages for the tutorial and to look nice when doing their thing. Now that this is done, the rest of the tutorial should be buildable at a somewhat faster pace. Hopefully I can get it all done tomorrow.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2A4AFAB-9C0C-4269-9BA8-598A8D079209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{310B1DCD-098A-4E0B-8AB2-208CBC846592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,9 +151,6 @@
     <t>lmb</t>
   </si>
   <si>
-    <t>Hold LMB to gather minerals</t>
-  </si>
-  <si>
     <t>Gather minerals</t>
   </si>
   <si>
@@ -377,29 +374,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Task: gather [number = enough minerals for fusion reactor] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00FFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>+minerals&amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -475,29 +449,6 @@
   </si>
   <si>
     <t>Firstly, we are going to need some building materials.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Please gather [number = enough minerals for fusion reactor] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00FFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>+minerals&amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
   </si>
   <si>
     <t>Good job! Any minerals you collect will be displayed here.</t>
@@ -728,6 +679,55 @@
   </si>
   <si>
     <t>Press D</t>
+  </si>
+  <si>
+    <t>Move the mouse over a mineral and hold down the left mouse button to mine it.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please gather 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00FFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+minerals&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Task: gather 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00FFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+minerals&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1241,8 +1241,8 @@
   <dimension ref="A1:AB983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1250,7 +1250,7 @@
     <col min="1" max="1" width="14.7109375" style="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="130.28515625" customWidth="1"/>
+    <col min="4" max="4" width="72.140625" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="102.28515625" customWidth="1"/>
   </cols>
@@ -1266,7 +1266,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -1316,16 +1316,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1334,16 +1334,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1352,16 +1352,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1370,16 +1370,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -1498,7 +1498,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10"/>
@@ -1514,7 +1514,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
@@ -1530,7 +1530,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
@@ -1582,7 +1582,7 @@
         <v>38</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
@@ -1598,7 +1598,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="9" t="s">
@@ -1616,13 +1616,13 @@
         <v>41</v>
       </c>
       <c r="D21" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="F21" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
@@ -1633,48 +1633,48 @@
         <v>30</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1701,16 +1701,16 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="9" t="s">
@@ -1719,36 +1719,36 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="9" t="s">
@@ -1757,190 +1757,190 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="9" t="s">
@@ -1949,84 +1949,84 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B41" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>77</v>
-      </c>
       <c r="D41" s="12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="11" t="s">
@@ -2035,36 +2035,36 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C44" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E44" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="6" t="s">
@@ -2073,68 +2073,68 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="E47" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="F47" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>91</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>92</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="9" t="s">
@@ -2143,94 +2143,94 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="E50" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="F50" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>98</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="34" t="s">
         <v>100</v>
-      </c>
-      <c r="D54" s="34" t="s">
-        <v>101</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="28"/>
       <c r="D55" s="13"/>
@@ -2239,176 +2239,176 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B56" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C56" s="28" t="s">
+      <c r="D56" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="7"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B57" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="28" t="s">
-        <v>103</v>
-      </c>
       <c r="D57" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B58" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C58" s="28" t="s">
-        <v>103</v>
-      </c>
       <c r="D58" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B59" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="28" t="s">
-        <v>103</v>
-      </c>
       <c r="D59" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B60" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="28" t="s">
-        <v>103</v>
-      </c>
       <c r="D60" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C61" s="28" t="s">
-        <v>103</v>
-      </c>
       <c r="D61" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B62" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C62" s="28" t="s">
-        <v>103</v>
-      </c>
       <c r="D62" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C63" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B64" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C66" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D66" s="12" t="s">
         <v>113</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>114</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="9"/>

</xml_diff>

<commit_message>
* Second stage of the tutorial is implemented * Added some extra minor functionality to facilitate that.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{310B1DCD-098A-4E0B-8AB2-208CBC846592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5DE92BF-12F3-456C-AB8A-3681B1221BB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="162">
   <si>
     <t>Stage</t>
   </si>
@@ -199,19 +199,10 @@
     <t>got power and water</t>
   </si>
   <si>
-    <t>build greenhouse</t>
-  </si>
-  <si>
     <t>Greenhouse appears and is buildable</t>
   </si>
   <si>
-    <t>build boiler</t>
-  </si>
-  <si>
     <t>Boiler appears and is buildable</t>
-  </si>
-  <si>
-    <t>build incinerator</t>
   </si>
   <si>
     <t>Incinerator appears and is buildable</t>
@@ -728,6 +719,21 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>enough for building</t>
+  </si>
+  <si>
+    <t>greenhouse</t>
+  </si>
+  <si>
+    <t>boiler</t>
+  </si>
+  <si>
+    <t>incinerator</t>
+  </si>
+  <si>
+    <t>ratios important</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1247,8 @@
   <dimension ref="A1:AB983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1266,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -1316,16 +1322,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1334,16 +1340,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1352,16 +1358,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1370,16 +1376,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -1498,7 +1504,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10"/>
@@ -1514,7 +1520,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
@@ -1530,7 +1536,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
@@ -1582,7 +1588,7 @@
         <v>38</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
@@ -1598,7 +1604,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="9" t="s">
@@ -1616,7 +1622,7 @@
         <v>41</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>42</v>
@@ -1636,7 +1642,7 @@
         <v>44</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="9" t="s">
@@ -1651,10 +1657,10 @@
         <v>30</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>47</v>
+        <v>157</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="7"/>
@@ -1670,7 +1676,7 @@
         <v>47</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7" t="s">
@@ -1710,7 +1716,7 @@
         <v>49</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="9" t="s">
@@ -1728,7 +1734,7 @@
         <v>50</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>51</v>
@@ -1748,7 +1754,7 @@
         <v>53</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="9" t="s">
@@ -1766,7 +1772,7 @@
         <v>54</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>55</v>
@@ -1786,7 +1792,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="7"/>
@@ -1799,14 +1805,14 @@
         <v>30</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
@@ -1817,14 +1823,14 @@
         <v>30</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
@@ -1835,14 +1841,14 @@
         <v>30</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>62</v>
+        <v>160</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1853,10 +1859,10 @@
         <v>30</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1869,10 +1875,10 @@
         <v>30</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="7"/>
@@ -1885,14 +1891,14 @@
         <v>30</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1903,14 +1909,14 @@
         <v>30</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1921,10 +1927,10 @@
         <v>30</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="7"/>
@@ -1937,10 +1943,10 @@
         <v>6</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="9" t="s">
@@ -1949,84 +1955,84 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>74</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="11" t="s">
@@ -2035,36 +2041,36 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="6" t="s">
@@ -2073,68 +2079,68 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="9" t="s">
@@ -2143,94 +2149,94 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F50" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D54" s="34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C55" s="28"/>
       <c r="D55" s="13"/>
@@ -2239,176 +2245,176 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="7"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B57" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D57" s="12" t="s">
         <v>101</v>
-      </c>
-      <c r="C57" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C58" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>105</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B64" s="27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="9"/>

</xml_diff>

<commit_message>
* Dialogue can now be progressed by clicking on the dialogue box or pressing z. Keep in mind the latter will progress all visible dialogue boxes that are marked as dismissable. * Got sick of being unable to just click stage all if the dialogue spreadsheet is open, so I added ~$Tutorial Dialogue.xlsx and its meta file to the git ignore, and from the look of it updating Tutorial Dialogue.xlsx and having Sourcetree register that it was changed remains unaffected.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5DE92BF-12F3-456C-AB8A-3681B1221BB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B1AEE3-4430-4546-95A9-EA8FBEF76E16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,9 +337,6 @@
     <t>If multiple lines of dialogue are listed with the same Dialogue Box ID and Dialogue Key, they'll be added to the same dialogue set and displayed in their dialogue box one after the other as the player indicates they've read each (except for the Console).</t>
   </si>
   <si>
-    <t>All dialogue is continued by pressing button [z]</t>
-  </si>
-  <si>
     <t>If dialogue needs to be separated into multiple lines, denote the line break with a ~.</t>
   </si>
   <si>
@@ -353,9 +350,6 @@
   </si>
   <si>
     <t>TODO</t>
-  </si>
-  <si>
-    <t>Juice: Typewriter FX</t>
   </si>
   <si>
     <t>Special characters are used to denote a section of dialogue as being coloured differently to the default for a given dialogue box. For reference, check the UI's DialogueBoxManager component.</t>
@@ -734,6 +728,12 @@
   </si>
   <si>
     <t>ratios important</t>
+  </si>
+  <si>
+    <t>Juice: Typewriter FX (might have already been covered by lerping of dialogue?)</t>
+  </si>
+  <si>
+    <t>All manually continuable dialogue is continued by pressing button [z] or clicking on the dialogue box.</t>
   </si>
 </sst>
 </file>
@@ -1247,8 +1247,8 @@
   <dimension ref="A1:AB983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1272,7 +1272,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -1322,16 +1322,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1340,16 +1340,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1358,16 +1358,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1376,16 +1376,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -1504,7 +1504,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10"/>
@@ -1520,7 +1520,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
@@ -1536,7 +1536,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
@@ -1588,7 +1588,7 @@
         <v>38</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
@@ -1604,7 +1604,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="9" t="s">
@@ -1622,7 +1622,7 @@
         <v>41</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>42</v>
@@ -1642,7 +1642,7 @@
         <v>44</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="9" t="s">
@@ -1657,10 +1657,10 @@
         <v>30</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="7"/>
@@ -1676,7 +1676,7 @@
         <v>47</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7" t="s">
@@ -1716,7 +1716,7 @@
         <v>49</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="9" t="s">
@@ -1734,7 +1734,7 @@
         <v>50</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>51</v>
@@ -1754,7 +1754,7 @@
         <v>53</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="9" t="s">
@@ -1772,7 +1772,7 @@
         <v>54</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>55</v>
@@ -1792,7 +1792,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="7"/>
@@ -1805,10 +1805,10 @@
         <v>30</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="7" t="s">
@@ -1823,10 +1823,10 @@
         <v>30</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="7" t="s">
@@ -1841,10 +1841,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="7" t="s">
@@ -1862,7 +1862,7 @@
         <v>61</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1878,7 +1878,7 @@
         <v>61</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="7"/>
@@ -1891,10 +1891,10 @@
         <v>30</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="7" t="s">
@@ -1912,7 +1912,7 @@
         <v>63</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
@@ -1930,7 +1930,7 @@
         <v>63</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="7"/>
@@ -1998,7 +1998,7 @@
         <v>73</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="10"/>
@@ -2014,7 +2014,7 @@
         <v>74</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="7" t="s">
@@ -2032,7 +2032,7 @@
         <v>76</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="11" t="s">
@@ -2050,7 +2050,7 @@
         <v>77</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>78</v>
@@ -2088,7 +2088,7 @@
         <v>82</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
@@ -2124,7 +2124,7 @@
         <v>86</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="7"/>
@@ -2178,7 +2178,7 @@
         <v>63</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="7"/>
@@ -2194,7 +2194,7 @@
         <v>63</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="7"/>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B55" s="28" t="s">
         <v>98</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B56" s="28" t="s">
         <v>98</v>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B57" s="15" t="s">
         <v>98</v>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B58" s="15" t="s">
         <v>98</v>
@@ -2293,7 +2293,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B59" s="15" t="s">
         <v>98</v>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B60" s="15" t="s">
         <v>98</v>
@@ -2318,14 +2318,14 @@
         <v>99</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B61" s="15" t="s">
         <v>98</v>
@@ -2334,14 +2334,14 @@
         <v>99</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B62" s="15" t="s">
         <v>98</v>
@@ -2350,71 +2350,71 @@
         <v>99</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B63" s="15" t="s">
         <v>98</v>
       </c>
       <c r="C63" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>107</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B64" s="27" t="s">
         <v>98</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B65" s="15" t="s">
         <v>98</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B66" s="15" t="s">
         <v>98</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="9"/>

</xml_diff>

<commit_message>
I think StageCombat is all done, just need to test it and do any required debugging, and make sure that aliens still spawn as they should outside of the tutorial.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B1AEE3-4430-4546-95A9-EA8FBEF76E16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9403CFD0-808C-453A-9E75-709E60095940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,28 +394,6 @@
         <family val="2"/>
       </rPr>
       <t>/Ice Drill\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Task: build a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;Turret&gt;</t>
     </r>
     <r>
       <rPr>
@@ -734,6 +712,37 @@
   </si>
   <si>
     <t>All manually continuable dialogue is continued by pressing button [z] or clicking on the dialogue box.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Task: build a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;Shotgun Turret&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;Machine Gun Turret&gt;.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1247,8 +1256,8 @@
   <dimension ref="A1:AB983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1322,16 +1331,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1340,16 +1349,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1358,16 +1367,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1376,16 +1385,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -1504,7 +1513,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10"/>
@@ -1520,7 +1529,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
@@ -1536,7 +1545,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
@@ -1588,7 +1597,7 @@
         <v>38</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
@@ -1604,7 +1613,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="9" t="s">
@@ -1622,7 +1631,7 @@
         <v>41</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>42</v>
@@ -1642,7 +1651,7 @@
         <v>44</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="9" t="s">
@@ -1657,10 +1666,10 @@
         <v>30</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="7"/>
@@ -1676,7 +1685,7 @@
         <v>47</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7" t="s">
@@ -1734,7 +1743,7 @@
         <v>50</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>51</v>
@@ -1772,7 +1781,7 @@
         <v>54</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>55</v>
@@ -1792,7 +1801,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="7"/>
@@ -1805,10 +1814,10 @@
         <v>30</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="7" t="s">
@@ -1823,10 +1832,10 @@
         <v>30</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="7" t="s">
@@ -1841,10 +1850,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="7" t="s">
@@ -1862,7 +1871,7 @@
         <v>61</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1878,7 +1887,7 @@
         <v>61</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="7"/>
@@ -1891,10 +1900,10 @@
         <v>30</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="7" t="s">
@@ -1912,7 +1921,7 @@
         <v>63</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
@@ -1930,7 +1939,7 @@
         <v>63</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="7"/>
@@ -1998,7 +2007,7 @@
         <v>73</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="10"/>
@@ -2014,7 +2023,7 @@
         <v>74</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="7" t="s">
@@ -2032,7 +2041,7 @@
         <v>76</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="11" t="s">
@@ -2050,7 +2059,7 @@
         <v>77</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>78</v>
@@ -2088,7 +2097,7 @@
         <v>82</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
@@ -2124,7 +2133,7 @@
         <v>86</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="7"/>
@@ -2178,7 +2187,7 @@
         <v>63</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="7"/>
@@ -2194,7 +2203,7 @@
         <v>63</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="7"/>
@@ -2318,7 +2327,7 @@
         <v>99</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="7"/>
@@ -2382,7 +2391,7 @@
         <v>105</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="7"/>
@@ -2414,7 +2423,7 @@
         <v>108</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="9"/>

</xml_diff>

<commit_message>
* Cleaned up dialogue so it doesn't scroll out past the confines of any of the text boxes, removed elipses because them scrolling onto a new line looks janky, and a couple of other small tweaks. * Moved StageManager out of the UI prefab because it just felt wrong for it to be in there rather than its own thing.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8661216C-9524-442D-81D1-11D9B7344594}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FC9C2F3-BAEA-473B-BFE4-9033F69B0559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,12 +19,11 @@
     <definedName name="P.O.Ds_first_steps">'Tutorial Dialogue'!$B$2:$F$22</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="176">
   <si>
     <t>Stage</t>
   </si>
@@ -50,18 +49,12 @@
     <t>ai online</t>
   </si>
   <si>
-    <t>Commencing system check . . .~AI unit: online.~Vitals: green.</t>
-  </si>
-  <si>
     <t>UI border appears, dialogue box Console appears in top left</t>
   </si>
   <si>
     <t>calibrate movement</t>
   </si>
   <si>
-    <t>Initialising movement system . . .~Movement calibration required.~Task: move using WASD.</t>
-  </si>
-  <si>
     <t>Prompt appears above POD (with transition in sem 2) with image showing how to move</t>
   </si>
   <si>
@@ -71,9 +64,6 @@
     <t>wasd</t>
   </si>
   <si>
-    <t>Move using WASD</t>
-  </si>
-  <si>
     <t>Move in each direction</t>
   </si>
   <si>
@@ -92,15 +82,9 @@
     <t>welcome pod</t>
   </si>
   <si>
-    <t>Connecting to S.E.E.R. . . .~Welcome Protective.Observation.Drone.</t>
-  </si>
-  <si>
     <t>planet livability</t>
   </si>
   <si>
-    <t>Initialising External Environment Scanner . . .~Planet P.R.I.M.E detected.~Launching planetlivability.exe . . .</t>
-  </si>
-  <si>
     <t>Clear Console first</t>
   </si>
   <si>
@@ -113,9 +97,6 @@
     <t>launch cat</t>
   </si>
   <si>
-    <t>Terraforming protocol updated.~Launching C.A.T.exe . . .</t>
-  </si>
-  <si>
     <t>CAT</t>
   </si>
   <si>
@@ -224,9 +205,6 @@
     <t>cat closed</t>
   </si>
   <si>
-    <t>C.A.T.exe has closed.</t>
-  </si>
-  <si>
     <t>Combat</t>
   </si>
   <si>
@@ -239,9 +217,6 @@
     <t>Triggered at night time; clear Console first</t>
   </si>
   <si>
-    <t>Launching D.O.G.exe . . .</t>
-  </si>
-  <si>
     <t>DOG</t>
   </si>
   <si>
@@ -275,9 +250,6 @@
     <t>shoot</t>
   </si>
   <si>
-    <t>Press space to shoot</t>
-  </si>
-  <si>
     <t>Shoot</t>
   </si>
   <si>
@@ -296,9 +268,6 @@
     <t>heal</t>
   </si>
   <si>
-    <t>Press E to heal</t>
-  </si>
-  <si>
     <t>Press E in range of the cryo egg</t>
   </si>
   <si>
@@ -306,9 +275,6 @@
   </si>
   <si>
     <t>dog closed</t>
-  </si>
-  <si>
-    <t>D.O.G.exe has closed.</t>
   </si>
   <si>
     <t>finished tutorial</t>
@@ -413,12 +379,6 @@
   </si>
   <si>
     <t>Good job! Any minerals you collect will be displayed here.</t>
-  </si>
-  <si>
-    <t>Perfect, this should be enough to construct your first building.</t>
-  </si>
-  <si>
-    <t>Stored in my memory are blueprints of buildings that can be used to convert this barren planet into a sustainable paradise for your humans in the cryo egg.</t>
   </si>
   <si>
     <r>
@@ -554,19 +514,10 @@
     <t>The more you build, the quicker you'll reach the end goal.</t>
   </si>
   <si>
-    <t>Make sure to keep the ratio between the buildings balanced, as going off balance can slow down your progress.</t>
-  </si>
-  <si>
     <t>Good luck and happy terraforming!</t>
   </si>
   <si>
-    <t>C.A.T. out. = ^__^ =</t>
-  </si>
-  <si>
     <t>DEFENCE ORGANISATION GUIDE ONLINE!</t>
-  </si>
-  <si>
-    <t>Listen up soldier! Those B.U.G.s look angry.</t>
   </si>
   <si>
     <r>
@@ -598,9 +549,6 @@
   </si>
   <si>
     <t>That's all you need to know. Good luck out there soldier! Don't die!</t>
-  </si>
-  <si>
-    <t>D.O.G. OUT!</t>
   </si>
   <si>
     <t>You don't need to put dialogue in quotation marks unless the character is using them in-line. Just type it as you want it presented in the dialogue box excepting the special characters for line breaks and colour tags.</t>
@@ -749,12 +697,6 @@
     <t>system check</t>
   </si>
   <si>
-    <t>Building system: ready.</t>
-  </si>
-  <si>
-    <t>External environment scanner: online.~Building system: enabled.~All systems are online.~Task: terraform this planet for human habitation. Begin.</t>
-  </si>
-  <si>
     <t>buildings ready</t>
   </si>
   <si>
@@ -767,15 +709,9 @@
     <t>clock gps inventory online</t>
   </si>
   <si>
-    <t>Commencing system check . . .</t>
-  </si>
-  <si>
     <t>initialising functions</t>
   </si>
   <si>
-    <t>AI unit: online.~Movement system: online and calibrated.~Vitals: green.~Initialising additional functionality . . .</t>
-  </si>
-  <si>
     <t>blank</t>
   </si>
   <si>
@@ -783,6 +719,72 @@
   </si>
   <si>
     <t>Console prints " " to initialise itself.</t>
+  </si>
+  <si>
+    <t>CAT.exe has closed.</t>
+  </si>
+  <si>
+    <t>Connecting to SEER.~Welcome Protective Observation Drone.</t>
+  </si>
+  <si>
+    <t>Initialising External Environment Scanner.~Planet PRIME detected.~Launching planetlivability.exe.</t>
+  </si>
+  <si>
+    <t>Terraforming protocol updated.~Launching CAT.exe.</t>
+  </si>
+  <si>
+    <t>CAT out. = ^__^ =</t>
+  </si>
+  <si>
+    <t>Launching DOG.exe.</t>
+  </si>
+  <si>
+    <t>DOG OUT!</t>
+  </si>
+  <si>
+    <t>DOG.exe has closed.</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>Commencing system check.~AI unit: online.~Vitals: green.</t>
+  </si>
+  <si>
+    <t>Initialising movement system.~Movement calibration required.~Task: move using the WASD keys.</t>
+  </si>
+  <si>
+    <t>Listen up soldier! Those BUGs look angry.</t>
+  </si>
+  <si>
+    <t>AI unit: online.~Movement system: online and calibrated.~Vitals: green.~Initialising additional functionality.</t>
+  </si>
+  <si>
+    <t>Press E to heal.</t>
+  </si>
+  <si>
+    <t>Press space to shoot.</t>
+  </si>
+  <si>
+    <t>Move using the WASD keys.~(Click this box or press Z to dismiss it.)</t>
+  </si>
+  <si>
+    <t>Construction system: ready.</t>
+  </si>
+  <si>
+    <t>External environment scanner: online.~Construction system: enabled.~All systems are online.~Task: terraform this planet for human habitation. Begin.</t>
+  </si>
+  <si>
+    <t>Make sure to keep the ratio between the buildings balanced; imbalance will slow down your progress.</t>
+  </si>
+  <si>
+    <t>Perfect, this should be enough to construct a building.</t>
+  </si>
+  <si>
+    <t>I have the blueprints of several that can help convert this rock into a paradise for the humans in the cryo egg.</t>
+  </si>
+  <si>
+    <t>Commencing system check.</t>
   </si>
 </sst>
 </file>
@@ -1300,9 +1302,9 @@
   </sheetPr>
   <dimension ref="A1:AB956"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1310,7 +1312,7 @@
     <col min="1" max="1" width="14.7109375" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.140625" customWidth="1"/>
+    <col min="4" max="4" width="213.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="102.28515625" customWidth="1"/>
   </cols>
@@ -1326,7 +1328,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -1346,11 +1348,11 @@
         <v>7</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1361,14 +1363,14 @@
         <v>6</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>11</v>
+        <v>164</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1376,16 +1378,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1394,16 +1396,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1412,16 +1414,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1430,16 +1432,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -1448,19 +1450,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="F8" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1471,14 +1473,14 @@
         <v>6</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1489,10 +1491,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>22</v>
+        <v>155</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
@@ -1505,14 +1507,14 @@
         <v>6</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>24</v>
+        <v>156</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1523,10 +1525,10 @@
         <v>6</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
@@ -1539,10 +1541,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>29</v>
+        <v>157</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="7"/>
@@ -1552,13 +1554,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10"/>
@@ -1568,13 +1570,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
@@ -1584,13 +1586,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
@@ -1603,14 +1605,14 @@
         <v>6</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
@@ -1621,14 +1623,14 @@
         <v>6</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
@@ -1636,13 +1638,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
@@ -1655,14 +1657,14 @@
         <v>6</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
@@ -1670,19 +1672,19 @@
         <v>5</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
@@ -1690,51 +1692,51 @@
         <v>5</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1761,791 +1763,791 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>66</v>
+        <v>154</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="24" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>90</v>
+        <v>167</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="37" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="37" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="37" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="D57" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="37" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D58" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="37" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D59" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="E59"/>
       <c r="F59"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="29" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="D60" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="F60" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C65" s="27" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="7"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="7"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B67" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C67" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D67" s="12" t="s">
         <v>97</v>
-      </c>
-      <c r="C67" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="E67" s="8"/>
       <c r="F67" s="7"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E68" s="8"/>
       <c r="F68" s="7"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="7"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="9"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="26" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="E71" s="8"/>
       <c r="F71" s="9"/>

</xml_diff>

<commit_message>
* Dialogue boxes add their text to the dialogue log. * Slight tweaks to StageControls to get the dialogue logging in the right order. * Adjustment to Dialogue Box to prevent breaking if Deactivate() would be called while it's tweening in. * Windmill base was missing it's material. * Cleaned out test file for loading dialogue from file.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FC9C2F3-BAEA-473B-BFE4-9033F69B0559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{02CCABE6-74C5-4D95-8FAB-A8EC67B32A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="176">
   <si>
     <t>Stage</t>
   </si>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t>launch dog</t>
-  </si>
-  <si>
-    <t>Warning! Hostile alien activity detected.</t>
   </si>
   <si>
     <t>Triggered at night time; clear Console first</t>
@@ -736,9 +733,6 @@
     <t>CAT out. = ^__^ =</t>
   </si>
   <si>
-    <t>Launching DOG.exe.</t>
-  </si>
-  <si>
     <t>DOG OUT!</t>
   </si>
   <si>
@@ -785,6 +779,12 @@
   </si>
   <si>
     <t>Commencing system check.</t>
+  </si>
+  <si>
+    <t>If you forget anything, press ESC and have a look in the pause menu.</t>
+  </si>
+  <si>
+    <t>Warning! Hostile alien activity detected.~Launching DOG.exe</t>
   </si>
 </sst>
 </file>
@@ -962,7 +962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1049,6 +1049,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1302,9 +1303,9 @@
   </sheetPr>
   <dimension ref="A1:AB956"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1328,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -1348,7 +1349,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
@@ -1366,7 +1367,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7" t="s">
@@ -1378,16 +1379,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1396,16 +1397,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1414,16 +1415,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1432,16 +1433,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -1456,7 +1457,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>13</v>
@@ -1494,7 +1495,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
@@ -1510,7 +1511,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="10" t="s">
@@ -1544,7 +1545,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="7"/>
@@ -1560,7 +1561,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10"/>
@@ -1576,7 +1577,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
@@ -1592,7 +1593,7 @@
         <v>25</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
@@ -1644,7 +1645,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
@@ -1660,7 +1661,7 @@
         <v>33</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="9" t="s">
@@ -1678,7 +1679,7 @@
         <v>35</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>36</v>
@@ -1698,7 +1699,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="9" t="s">
@@ -1713,10 +1714,10 @@
         <v>24</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="7"/>
@@ -1732,7 +1733,7 @@
         <v>41</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7" t="s">
@@ -1772,7 +1773,7 @@
         <v>43</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="9" t="s">
@@ -1790,7 +1791,7 @@
         <v>44</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>45</v>
@@ -1810,7 +1811,7 @@
         <v>47</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="9" t="s">
@@ -1828,7 +1829,7 @@
         <v>48</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>49</v>
@@ -1848,7 +1849,7 @@
         <v>51</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="7"/>
@@ -1861,10 +1862,10 @@
         <v>24</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="7" t="s">
@@ -1879,10 +1880,10 @@
         <v>24</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="7" t="s">
@@ -1897,10 +1898,10 @@
         <v>24</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="7" t="s">
@@ -1918,7 +1919,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1934,28 +1935,24 @@
         <v>55</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="20" t="s">
-        <v>40</v>
-      </c>
+    <row r="35" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="20"/>
       <c r="B35" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
@@ -1964,15 +1961,15 @@
       <c r="B36" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="32" t="s">
-        <v>114</v>
+      <c r="C36" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="38" t="s">
+        <v>174</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1985,46 +1982,46 @@
       <c r="C37" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="7"/>
+      <c r="D37" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="7" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="16" t="s">
-        <v>6</v>
+      <c r="B38" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="F38" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="22" t="s">
-        <v>60</v>
+      <c r="A39" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>62</v>
+        <v>153</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="9" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2038,23 +2035,25 @@
         <v>61</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="7"/>
+        <v>175</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
         <v>60</v>
       </c>
       <c r="B41" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>65</v>
-      </c>
       <c r="D41" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="10"/>
@@ -2064,17 +2063,17 @@
         <v>60</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2085,10 +2084,10 @@
         <v>6</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="11" t="s">
@@ -2100,19 +2099,19 @@
         <v>60</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C44" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D44" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E44" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2123,10 +2122,10 @@
         <v>6</v>
       </c>
       <c r="C45" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="6" t="s">
@@ -2138,13 +2137,13 @@
         <v>60</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
@@ -2157,16 +2156,16 @@
         <v>11</v>
       </c>
       <c r="C47" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D47" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E47" s="6" t="s">
+      <c r="F47" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2174,13 +2173,13 @@
         <v>60</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="7"/>
@@ -2193,10 +2192,10 @@
         <v>6</v>
       </c>
       <c r="C49" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>79</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="9" t="s">
@@ -2211,16 +2210,16 @@
         <v>11</v>
       </c>
       <c r="C50" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D50" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="E50" s="6" t="s">
+      <c r="F50" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2228,13 +2227,13 @@
         <v>60</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>57</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="7"/>
@@ -2244,13 +2243,13 @@
         <v>60</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>57</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="7"/>
@@ -2263,10 +2262,10 @@
         <v>6</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="7"/>
@@ -2279,275 +2278,275 @@
         <v>11</v>
       </c>
       <c r="C54" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="32" t="s">
         <v>84</v>
-      </c>
-      <c r="D54" s="32" t="s">
-        <v>85</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D58" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D59" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E59"/>
       <c r="F59"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="29" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B60" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C60" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D60" t="s">
         <v>151</v>
       </c>
-      <c r="D60" t="s">
+      <c r="F60" t="s">
         <v>152</v>
-      </c>
-      <c r="F60" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B61" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C61" s="27" t="s">
+      <c r="D61" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>88</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B62" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C62" s="27" t="s">
-        <v>87</v>
-      </c>
       <c r="D62" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B63" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C63" s="27" t="s">
-        <v>87</v>
-      </c>
       <c r="D63" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B64" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C64" s="27" t="s">
-        <v>87</v>
-      </c>
       <c r="D64" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B65" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="27" t="s">
-        <v>87</v>
-      </c>
       <c r="D65" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="7"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B66" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C66" s="27" t="s">
-        <v>87</v>
-      </c>
       <c r="D66" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="7"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B67" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="27" t="s">
-        <v>87</v>
-      </c>
       <c r="D67" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E67" s="8"/>
       <c r="F67" s="7"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C68" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D68" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>94</v>
       </c>
       <c r="E68" s="8"/>
       <c r="F68" s="7"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="7"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="9"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E71" s="8"/>
       <c r="F71" s="9"/>
@@ -8753,9 +8752,9 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:A53">
+  <conditionalFormatting sqref="A40:A53">
     <cfRule type="containsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(A39))=0</formula>
+      <formula>LEN(TRIM(A40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">

</xml_diff>

<commit_message>
* Tutorial speeding up for bringing UI elements in in-code * Tutorial refactoring to separate different sections within a stage * Condensing dialogue sets that are merely called one line after the next for the same dialogue box (i.e. the console) as a result of the refactoring
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0558A6A6-C0C5-4D63-9422-38DA81314FDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9545E08-A2D9-4A49-855E-338F3F3BC07F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13815" yWindow="6510" windowWidth="14745" windowHeight="7815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial Dialogue" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="P.O.Ds_first_steps">'Tutorial Dialogue'!$B$2:$F$22</definedName>
+    <definedName name="P.O.Ds_first_steps">'Tutorial Dialogue'!$B$2:$F$21</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="168">
   <si>
     <t>Stage</t>
   </si>
@@ -73,13 +73,7 @@
     <t>systems online</t>
   </si>
   <si>
-    <t>Movement calibrated.~System check complete.~All systems online.</t>
-  </si>
-  <si>
     <t>Prompt closes</t>
-  </si>
-  <si>
-    <t>welcome pod</t>
   </si>
   <si>
     <t>planet livability</t>
@@ -549,21 +543,9 @@
     <t>system check</t>
   </si>
   <si>
-    <t>buildings ready</t>
-  </si>
-  <si>
     <t>begin game</t>
   </si>
   <si>
-    <t>Chronometer: online.~GPS: online.~Inventory: online.</t>
-  </si>
-  <si>
-    <t>clock gps inventory online</t>
-  </si>
-  <si>
-    <t>initialising functions</t>
-  </si>
-  <si>
     <t>blank</t>
   </si>
   <si>
@@ -576,9 +558,6 @@
     <t>CAT.exe has closed.</t>
   </si>
   <si>
-    <t>Connecting to SEER.~Welcome Protective Observation Drone.</t>
-  </si>
-  <si>
     <t>Initialising External Environment Scanner.~Planet PRIME detected.~Launching planetlivability.exe.</t>
   </si>
   <si>
@@ -606,9 +585,6 @@
     <t>Listen up soldier! Those BUGs look angry.</t>
   </si>
   <si>
-    <t>AI unit: online.~Movement system: online and calibrated.~Vitals: green.~Initialising additional functionality.</t>
-  </si>
-  <si>
     <t>Press E to heal.</t>
   </si>
   <si>
@@ -618,12 +594,6 @@
     <t>Move using the WASD keys.~(Click this box or press Z to dismiss it.)</t>
   </si>
   <si>
-    <t>Construction system: ready.</t>
-  </si>
-  <si>
-    <t>External environment scanner: online.~Construction system: enabled.~All systems are online.~Task: terraform this planet for human habitation. Begin.</t>
-  </si>
-  <si>
     <t>Make sure to keep the ratio between the buildings balanced; imbalance will slow down your progress.</t>
   </si>
   <si>
@@ -631,9 +601,6 @@
   </si>
   <si>
     <t>I have the blueprints of several that can help convert this rock into a paradise for the humans in the cryo egg.</t>
-  </si>
-  <si>
-    <t>Commencing system check.</t>
   </si>
   <si>
     <t>If you forget anything, press ESC and have a look in the pause menu.</t>
@@ -776,6 +743,15 @@
       </rPr>
       <t>, it turns water into oxygen for your humans to breathe.</t>
     </r>
+  </si>
+  <si>
+    <t>Construction system: online.~External environment scanner: online.~Construction system: enabled.~All systems are online.~Task: terraform this planet for human habitation. Begin.</t>
+  </si>
+  <si>
+    <t>Commencing system check.~AI unit: online.~Movement system: online and calibrated.~Vitals: green.~Chronometer: online.~GPS: online.~Inventory: online.</t>
+  </si>
+  <si>
+    <t>Movement calibrated.~Connecting to SEER.~System check complete.~All systems online.~Welcome Protective Observation Drone.</t>
   </si>
 </sst>
 </file>
@@ -1287,11 +1263,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB956"/>
+  <dimension ref="A1:AB952"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1315,7 +1291,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -1335,7 +1311,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
@@ -1353,7 +1329,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7" t="s">
@@ -1365,16 +1341,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1383,16 +1359,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1401,16 +1377,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1419,16 +1395,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -1443,7 +1419,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>13</v>
@@ -1463,11 +1439,11 @@
         <v>15</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>16</v>
+        <v>167</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1478,13 +1454,15 @@
         <v>6</v>
       </c>
       <c r="C10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
@@ -1496,13 +1474,11 @@
       <c r="C11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>149</v>
+      <c r="D11" s="31" t="s">
+        <v>20</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
@@ -1514,8 +1490,8 @@
       <c r="C12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="31" t="s">
-        <v>22</v>
+      <c r="D12" s="30" t="s">
+        <v>143</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
@@ -1524,46 +1500,46 @@
       <c r="A13" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>6</v>
+      <c r="B13" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="10"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
@@ -1572,17 +1548,19 @@
       <c r="A16" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="D16" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>101</v>
-      </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
@@ -1592,366 +1570,366 @@
         <v>6</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>6</v>
+      <c r="B18" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="F18" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>24</v>
+      <c r="B19" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C19" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>6</v>
+      <c r="B20" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>34</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>11</v>
+      <c r="B21" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
-        <v>5</v>
+      <c r="A22" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="9" t="s">
-        <v>39</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="7"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>24</v>
+        <v>38</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="30" t="s">
-        <v>166</v>
+      <c r="D24" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="E24" s="6"/>
-      <c r="F24" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
-      <c r="AA24" s="3"/>
-      <c r="AB24" s="3"/>
+      <c r="F24" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>6</v>
+        <v>38</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="C25" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="9" t="s">
-        <v>20</v>
+      <c r="F25" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>24</v>
+        <v>38</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="E26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>46</v>
+      <c r="D26" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>6</v>
+        <v>38</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="C27" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="9" t="s">
-        <v>20</v>
+      <c r="F27" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>50</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E29" s="8"/>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>170</v>
+        <v>53</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>103</v>
       </c>
       <c r="E32" s="8"/>
-      <c r="F32" s="7" t="s">
-        <v>54</v>
-      </c>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="20"/>
       <c r="B34" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="B35" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="D35" s="32" t="s">
-        <v>164</v>
+        <v>22</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>157</v>
       </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="D36" s="38" t="s">
-        <v>168</v>
+        <v>22</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>105</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
@@ -1960,41 +1938,41 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="7" t="s">
-        <v>58</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>24</v>
+        <v>38</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>57</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="F38" s="7"/>
+      <c r="F38" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="20" t="s">
-        <v>40</v>
+      <c r="A39" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>6</v>
@@ -2003,539 +1981,507 @@
         <v>59</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="9" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>6</v>
+        <v>58</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="9" t="s">
-        <v>62</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="10"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B41" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="D41" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>65</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="7" t="s">
-        <v>66</v>
+        <v>134</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>6</v>
+        <v>58</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="C43" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D43" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="11" t="s">
-        <v>34</v>
+      <c r="F43" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="23" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>69</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E44" s="8"/>
       <c r="F44" s="6" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>6</v>
+      <c r="A45" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B46" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="17" t="s">
+      <c r="F46" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="E47" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="D47" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="7"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C48" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="12" t="s">
-        <v>111</v>
-      </c>
       <c r="E48" s="8"/>
-      <c r="F48" s="7"/>
+      <c r="F48" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>6</v>
+        <v>58</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="9" t="s">
-        <v>34</v>
+      <c r="F49" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="B50" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>81</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E50" s="8"/>
+      <c r="F50" s="7"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>112</v>
+        <v>55</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>145</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>152</v>
+        <v>80</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="E53" s="8"/>
-      <c r="F53" s="7"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D54" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C54" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="D55" s="30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="37" t="s">
         <v>137</v>
+      </c>
+      <c r="D55" t="s">
+        <v>165</v>
+      </c>
+      <c r="E55"/>
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="29" t="s">
+        <v>147</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="D56" s="30" t="s">
-        <v>158</v>
+        <v>138</v>
+      </c>
+      <c r="D56" t="s">
+        <v>139</v>
+      </c>
+      <c r="F56" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="D57" t="s">
-        <v>141</v>
-      </c>
+      <c r="A57" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="D58" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="D59" t="s">
-        <v>163</v>
-      </c>
-      <c r="E59"/>
-      <c r="F59"/>
+      <c r="A58" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" s="8"/>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="8"/>
+      <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="D60" t="s">
-        <v>145</v>
-      </c>
-      <c r="F60" t="s">
-        <v>146</v>
-      </c>
+      <c r="A60" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E60" s="8"/>
+      <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="27" t="s">
-        <v>85</v>
+        <v>96</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>87</v>
+        <v>133</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C64" s="27" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C65" s="27" t="s">
-        <v>86</v>
+        <v>96</v>
+      </c>
+      <c r="B65" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="7"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C66" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>91</v>
+        <v>83</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="E66" s="8"/>
-      <c r="F66" s="7"/>
+      <c r="F66" s="9"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C67" s="27" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="E67" s="8"/>
-      <c r="F67" s="7"/>
+      <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E68" s="8"/>
-      <c r="F68" s="7"/>
+      <c r="A68" s="28"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="4"/>
+      <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B69" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="C69" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E69" s="8"/>
-      <c r="F69" s="7"/>
+      <c r="A69" s="28"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="4"/>
+      <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="9"/>
+      <c r="A70" s="28"/>
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="4"/>
+      <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C71" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E71" s="8"/>
-      <c r="F71" s="9"/>
+      <c r="A71" s="28"/>
+      <c r="B71" s="28"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="4"/>
+      <c r="F71" s="2"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="28"/>
@@ -8704,48 +8650,20 @@
       <c r="D952" s="4"/>
       <c r="F952" s="2"/>
     </row>
-    <row r="953" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A953" s="28"/>
-      <c r="B953" s="28"/>
-      <c r="C953" s="28"/>
-      <c r="D953" s="4"/>
-      <c r="F953" s="2"/>
-    </row>
-    <row r="954" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A954" s="28"/>
-      <c r="B954" s="28"/>
-      <c r="C954" s="28"/>
-      <c r="D954" s="4"/>
-      <c r="F954" s="2"/>
-    </row>
-    <row r="955" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A955" s="28"/>
-      <c r="B955" s="28"/>
-      <c r="C955" s="28"/>
-      <c r="D955" s="4"/>
-      <c r="F955" s="2"/>
-    </row>
-    <row r="956" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A956" s="28"/>
-      <c r="B956" s="28"/>
-      <c r="C956" s="28"/>
-      <c r="D956" s="4"/>
-      <c r="F956" s="2"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AB1">
     <cfRule type="notContainsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40:A53">
+  <conditionalFormatting sqref="A39:A52">
     <cfRule type="containsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(A40))=0</formula>
+      <formula>LEN(TRIM(A39))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
+  <conditionalFormatting sqref="A53">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A54))=0</formula>
+      <formula>LEN(TRIM(A53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>

<commit_message>
* Forgot to make non-turret building buttons non-interactable during the combat stage. * Adjusted stages to make building buttons uninteractable during the tutorial if enough of a building has been placed to do what the tutorial needs, even if it's still in the middle of being built. For StageCombat, this includes fusion reactors if the player needs more power to build a shotgun turret and a machine gun turret.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9545E08-A2D9-4A49-855E-338F3F3BC07F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB2C7B6A-B632-42FB-8968-1B9E6B899411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13815" yWindow="6510" windowWidth="14745" windowHeight="7815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial Dialogue" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="P.O.Ds_first_steps">'Tutorial Dialogue'!$B$2:$F$21</definedName>
+    <definedName name="P.O.Ds_first_steps">'Tutorial Dialogue'!$B$2:$F$19</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="163">
   <si>
     <t>Stage</t>
   </si>
@@ -82,12 +82,6 @@
     <t>Clear Console first</t>
   </si>
   <si>
-    <t>planet unlivable</t>
-  </si>
-  <si>
-    <t>&lt;PLANET IS UNABLE TO SUPPORT LIFE.&gt;</t>
-  </si>
-  <si>
     <t>launch cat</t>
   </si>
   <si>
@@ -97,22 +91,7 @@
     <t>need minerals</t>
   </si>
   <si>
-    <t>scan minerals</t>
-  </si>
-  <si>
-    <t>Scanning for mineral deposits.</t>
-  </si>
-  <si>
     <t>Minimap Appears</t>
-  </si>
-  <si>
-    <t>minerals detected</t>
-  </si>
-  <si>
-    <t>Minerals detected.</t>
-  </si>
-  <si>
-    <t>Minimap Detection + Mineral Layer (Minimap detection has layers)</t>
   </si>
   <si>
     <t>gather minerals</t>
@@ -561,9 +540,6 @@
     <t>Initialising External Environment Scanner.~Planet PRIME detected.~Launching planetlivability.exe.</t>
   </si>
   <si>
-    <t>Terraforming protocol updated.~Launching CAT.exe.</t>
-  </si>
-  <si>
     <t>CAT out. = ^__^ =</t>
   </si>
   <si>
@@ -752,6 +728,15 @@
   </si>
   <si>
     <t>Movement calibrated.~Connecting to SEER.~System check complete.~All systems online.~Welcome Protective Observation Drone.</t>
+  </si>
+  <si>
+    <t>Scanning for mineral deposits.~Minerals detected.</t>
+  </si>
+  <si>
+    <t>detect minerals</t>
+  </si>
+  <si>
+    <t>&lt;PLANET IS UNABLE TO SUPPORT LIFE.&gt;~Terraforming protocol updated.~Launching CAT.exe.</t>
   </si>
 </sst>
 </file>
@@ -1263,11 +1248,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB952"/>
+  <dimension ref="A1:AB950"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1291,7 +1276,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -1311,7 +1296,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
@@ -1329,7 +1314,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7" t="s">
@@ -1341,16 +1326,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1359,16 +1344,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1377,16 +1362,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1395,16 +1380,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -1419,7 +1404,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>13</v>
@@ -1439,7 +1424,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="7" t="s">
@@ -1457,7 +1442,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="10" t="s">
@@ -1475,7 +1460,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>20</v>
+        <v>162</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
@@ -1484,46 +1469,46 @@
       <c r="A12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>6</v>
+      <c r="B12" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>143</v>
+        <v>90</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
@@ -1532,35 +1517,35 @@
       <c r="A15" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>6</v>
+      <c r="B16" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>25</v>
+        <v>118</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
@@ -1570,156 +1555,160 @@
         <v>6</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="7" t="s">
-        <v>29</v>
+      <c r="F17" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>22</v>
+      <c r="B18" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
+        <v>117</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>6</v>
+      <c r="B19" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="D21" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="E23" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="F23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>41</v>
-      </c>
       <c r="D24" s="12" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="9" t="s">
@@ -1728,732 +1717,708 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>47</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="E27" s="8"/>
       <c r="F27" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>101</v>
+        <v>156</v>
       </c>
       <c r="E28" s="8"/>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>164</v>
+        <v>46</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>96</v>
       </c>
       <c r="E30" s="8"/>
-      <c r="F30" s="7" t="s">
-        <v>51</v>
-      </c>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>159</v>
+        <v>46</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>97</v>
       </c>
       <c r="E31" s="8"/>
-      <c r="F31" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="s">
-        <v>38</v>
-      </c>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="20"/>
       <c r="B32" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="32" t="s">
-        <v>104</v>
+        <v>20</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>149</v>
       </c>
       <c r="E33" s="8"/>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
+      <c r="F33" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="20" t="s">
+        <v>31</v>
+      </c>
       <c r="B34" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>131</v>
+        <v>48</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="E34" s="8"/>
-      <c r="F34" s="7"/>
+      <c r="F34" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="D35" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="7" t="s">
-        <v>54</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C36" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>57</v>
-      </c>
       <c r="D38" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="9" t="s">
-        <v>32</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="10"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>6</v>
+        <v>51</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="9" t="s">
-        <v>60</v>
+        <v>142</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>62</v>
-      </c>
       <c r="D40" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="10"/>
+        <v>127</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B41" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="11" t="s">
-        <v>32</v>
+        <v>63</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>61</v>
+      <c r="A43" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>54</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>68</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>6</v>
+        <v>51</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="6" t="s">
-        <v>32</v>
+        <v>64</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="25" t="s">
-        <v>61</v>
+      <c r="A45" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>108</v>
+        <v>67</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
+      <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>11</v>
+        <v>51</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B47" s="23" t="s">
-        <v>61</v>
+        <v>51</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>6</v>
+        <v>51</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>76</v>
+        <v>48</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="E48" s="8"/>
-      <c r="F48" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="18" t="s">
-        <v>11</v>
+        <v>51</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="7"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" s="23" t="s">
-        <v>61</v>
+        <v>51</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="7"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>61</v>
+        <v>51</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="D51" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="22" t="s">
-        <v>58</v>
+      <c r="A52" s="37" t="s">
+        <v>128</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E52" s="8"/>
-      <c r="F52" s="7"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
+      <c r="C52" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="D53" t="s">
+        <v>157</v>
+      </c>
+      <c r="E53"/>
+      <c r="F53"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="37" t="s">
-        <v>135</v>
+      <c r="A54" s="29" t="s">
+        <v>139</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D54" s="30" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="D55" t="s">
-        <v>165</v>
-      </c>
-      <c r="E55"/>
-      <c r="F55"/>
+        <v>131</v>
+      </c>
+      <c r="D54" t="s">
+        <v>132</v>
+      </c>
+      <c r="F54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="8"/>
+      <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="D56" t="s">
-        <v>139</v>
-      </c>
-      <c r="F56" t="s">
-        <v>140</v>
-      </c>
+      <c r="A56" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E56" s="8"/>
+      <c r="F56" s="7"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B57" s="27" t="s">
-        <v>83</v>
+        <v>89</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>76</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="26" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="26" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="26" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="26" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>133</v>
+        <v>87</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="26" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B62" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C62" s="27" t="s">
+      <c r="D62" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B63" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="27" t="s">
-        <v>84</v>
-      </c>
       <c r="D63" s="12" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="26" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B64" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C64" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>91</v>
+      <c r="D64" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="E64" s="8"/>
-      <c r="F64" s="7"/>
+      <c r="F64" s="9"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B65" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C65" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>86</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="E65" s="8"/>
-      <c r="F65" s="7"/>
+      <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D66" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E66" s="8"/>
-      <c r="F66" s="9"/>
+      <c r="A66" s="28"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="4"/>
+      <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E67" s="8"/>
-      <c r="F67" s="9"/>
+      <c r="A67" s="28"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="4"/>
+      <c r="F67" s="2"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="28"/>
@@ -8636,34 +8601,20 @@
       <c r="D950" s="4"/>
       <c r="F950" s="2"/>
     </row>
-    <row r="951" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A951" s="28"/>
-      <c r="B951" s="28"/>
-      <c r="C951" s="28"/>
-      <c r="D951" s="4"/>
-      <c r="F951" s="2"/>
-    </row>
-    <row r="952" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A952" s="28"/>
-      <c r="B952" s="28"/>
-      <c r="C952" s="28"/>
-      <c r="D952" s="4"/>
-      <c r="F952" s="2"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AB1">
     <cfRule type="notContainsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:A52">
+  <conditionalFormatting sqref="A37:A50">
     <cfRule type="containsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(A39))=0</formula>
+      <formula>LEN(TRIM(A37))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
+  <conditionalFormatting sqref="A51">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A53))=0</formula>
+      <formula>LEN(TRIM(A51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>

<commit_message>
Forgot to remove some old dialogue calls from StageSkipTutorial
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB2C7B6A-B632-42FB-8968-1B9E6B899411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{618A7696-1D0F-4919-A634-7FB9E4260C6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial Dialogue" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated the progress-dialogue hotkey, though E is already taken for healing so I changed it to Q. Either could be updated if we think it necessary after testing.
</commit_message>
<xml_diff>
--- a/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
+++ b/Assets/Resources/Dialogue/Tutorial Dialogue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\Unity\POD\Assets\Resources\Dialogue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{618A7696-1D0F-4919-A634-7FB9E4260C6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{118CA611-2F50-4AB4-A09E-BFB592FC99C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial Dialogue" sheetId="1" r:id="rId1"/>
@@ -480,9 +480,6 @@
   </si>
   <si>
     <t>Juice: Typewriter FX (might have already been covered by lerping of dialogue?)</t>
-  </si>
-  <si>
-    <t>All manually continuable dialogue is continued by pressing button [z] or clicking on the dialogue box.</t>
   </si>
   <si>
     <r>
@@ -567,9 +564,6 @@
     <t>Press space to shoot.</t>
   </si>
   <si>
-    <t>Move using the WASD keys.~(Click this box or press Z to dismiss it.)</t>
-  </si>
-  <si>
     <t>Make sure to keep the ratio between the buildings balanced; imbalance will slow down your progress.</t>
   </si>
   <si>
@@ -737,6 +731,12 @@
   </si>
   <si>
     <t>&lt;PLANET IS UNABLE TO SUPPORT LIFE.&gt;~Terraforming protocol updated.~Launching CAT.exe.</t>
+  </si>
+  <si>
+    <t>Move using the WASD keys.~(Click this box or press Q to dismiss it.)</t>
+  </si>
+  <si>
+    <t>All manually continuable dialogue is continued by pressing button [Q] or clicking on the dialogue box.</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1252,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1296,7 +1296,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
@@ -1314,7 +1314,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7" t="s">
@@ -1404,7 +1404,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>13</v>
@@ -1424,7 +1424,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="7" t="s">
@@ -1442,7 +1442,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="10" t="s">
@@ -1460,7 +1460,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
@@ -1521,10 +1521,10 @@
         <v>6</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7" t="s">
@@ -1614,7 +1614,7 @@
         <v>120</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="7"/>
@@ -1630,7 +1630,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="7" t="s">
@@ -1670,7 +1670,7 @@
         <v>34</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="9" t="s">
@@ -1688,7 +1688,7 @@
         <v>35</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>36</v>
@@ -1708,7 +1708,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="9" t="s">
@@ -1726,7 +1726,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>40</v>
@@ -1780,7 +1780,7 @@
         <v>122</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="7" t="s">
@@ -1798,7 +1798,7 @@
         <v>123</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="7" t="s">
@@ -1846,7 +1846,7 @@
         <v>124</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="7"/>
@@ -1862,7 +1862,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="7" t="s">
@@ -1898,7 +1898,7 @@
         <v>48</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="7"/>
@@ -1914,7 +1914,7 @@
         <v>50</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="9" t="s">
@@ -1932,7 +1932,7 @@
         <v>52</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="9" t="s">
@@ -1966,7 +1966,7 @@
         <v>56</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="7" t="s">
@@ -1984,7 +1984,7 @@
         <v>58</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="11" t="s">
@@ -2056,7 +2056,7 @@
         <v>64</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>65</v>
@@ -2110,7 +2110,7 @@
         <v>70</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>71</v>
@@ -2146,7 +2146,7 @@
         <v>48</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="7"/>
@@ -2162,7 +2162,7 @@
         <v>73</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="7"/>
@@ -2185,49 +2185,49 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D52" s="30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D53" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E53"/>
       <c r="F53"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C54" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="D54" t="s">
         <v>131</v>
       </c>
-      <c r="D54" t="s">
+      <c r="F54" t="s">
         <v>132</v>
-      </c>
-      <c r="F54" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2305,7 +2305,7 @@
         <v>77</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="7"/>

</xml_diff>